<commit_message>
Add image carousel functionality and update registro_herramientas.txt with new tool selections
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inacapmailcl-my.sharepoint.com/personal/juan_erices04_inacapmail_cl/Documents/Desktop/acceso_panol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_946C8F9C91F7436719BEC114DF8008236A665B42" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3D6D1A9-AA8E-4ECF-BCBD-85EBDA245DF4}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="11_946C8F9C91F7436719BEC114DF8008236A665B42" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD4928A7-D135-4BCC-B080-75FA3920E5E0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Análisis</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Herramientas</t>
+  </si>
+  <si>
+    <t>Sierra electrica</t>
   </si>
 </sst>
 </file>
@@ -289,8 +292,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FAA71FDA-3F3B-413C-A6A9-32E16306DA2F}" name="Tabla1" displayName="Tabla1" ref="A1:B54" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B54" xr:uid="{FAA71FDA-3F3B-413C-A6A9-32E16306DA2F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FAA71FDA-3F3B-413C-A6A9-32E16306DA2F}" name="Tabla1" displayName="Tabla1" ref="A1:B55" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B55" xr:uid="{FAA71FDA-3F3B-413C-A6A9-32E16306DA2F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5F3CBBF7-F94A-4689-9042-4369A8D2F49F}" name="Categoria"/>
     <tableColumn id="2" xr3:uid="{CD7582D6-A22E-4140-900D-99A273CCC885}" name="Herramientas"/>
@@ -500,10 +503,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection sqref="A1:B54"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -690,85 +693,86 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>54</v>
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>55</v>
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>56</v>
       </c>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>37</v>
       </c>
@@ -807,6 +811,11 @@
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>